<commit_message>
Planning et UML à jour, RP_Richoz terminé
</commit_message>
<xml_diff>
--- a/133_GESTPROJ_RICHOZ_Matteo_MORISETTI_David.xlsx
+++ b/133_GESTPROJ_RICHOZ_Matteo_MORISETTI_David.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eduetatfr-my.sharepoint.com/personal/david_morisetti_studentfr_ch/Documents/Module 133/133_projet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="145" documentId="13_ncr:1_{842784B3-AB82-49D3-8E72-B8CBCF326D84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE5BD29D-204D-4190-88F5-A98ED29B9556}"/>
+  <xr:revisionPtr revIDLastSave="149" documentId="13_ncr:1_{842784B3-AB82-49D3-8E72-B8CBCF326D84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB5D8603-1E43-49AA-AC39-E8D5D9494D05}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning" sheetId="1" r:id="rId1"/>
@@ -942,44 +942,44 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -996,10 +996,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1294,8 +1290,8 @@
   </sheetPr>
   <dimension ref="A1:Q27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q22" sqref="Q22"/>
+    <sheetView showGridLines="0" view="pageLayout" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7.85546875" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1306,64 +1302,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="42"/>
-      <c r="M1" s="42"/>
-      <c r="N1" s="42"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="53"/>
+      <c r="N1" s="53"/>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:17" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="45"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="46"/>
       <c r="L3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M3" s="43">
+      <c r="M3" s="45">
         <v>300232</v>
       </c>
-      <c r="N3" s="45"/>
+      <c r="N3" s="46"/>
     </row>
     <row r="4" spans="1:17" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="43" t="s">
+      <c r="B4" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
-      <c r="H4" s="44"/>
-      <c r="I4" s="44"/>
-      <c r="J4" s="44"/>
-      <c r="K4" s="45"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="54"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="54"/>
+      <c r="J4" s="54"/>
+      <c r="K4" s="46"/>
       <c r="L4" s="2" t="s">
         <v>3</v>
       </c>
@@ -1373,32 +1369,32 @@
     </row>
     <row r="6" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="47"/>
-      <c r="D7" s="48"/>
-      <c r="E7" s="46" t="s">
+      <c r="C7" s="43"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="47"/>
-      <c r="G7" s="48"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="44"/>
       <c r="H7" s="16"/>
-      <c r="I7" s="46" t="s">
+      <c r="I7" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="J7" s="47"/>
-      <c r="K7" s="48"/>
-      <c r="L7" s="46" t="s">
+      <c r="J7" s="43"/>
+      <c r="K7" s="44"/>
+      <c r="L7" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="M7" s="47"/>
-      <c r="N7" s="48"/>
-      <c r="O7" s="46" t="s">
+      <c r="M7" s="43"/>
+      <c r="N7" s="44"/>
+      <c r="O7" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="P7" s="47"/>
-      <c r="Q7" s="48"/>
+      <c r="P7" s="43"/>
+      <c r="Q7" s="44"/>
     </row>
     <row r="8" spans="1:17" s="1" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="36" t="s">
@@ -1467,13 +1463,13 @@
       <c r="E9" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="F9" s="49" t="s">
+      <c r="F9" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="49" t="s">
+      <c r="G9" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="H9" s="52" t="s">
+      <c r="H9" s="50" t="s">
         <v>24</v>
       </c>
       <c r="I9" s="11"/>
@@ -1494,9 +1490,9 @@
       <c r="C10" s="6"/>
       <c r="D10" s="12"/>
       <c r="E10" s="11"/>
-      <c r="F10" s="50"/>
-      <c r="G10" s="50"/>
-      <c r="H10" s="53"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="48"/>
+      <c r="H10" s="51"/>
       <c r="I10" s="11"/>
       <c r="J10" s="6"/>
       <c r="K10" s="12"/>
@@ -1517,9 +1513,9 @@
       <c r="E11" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="F11" s="50"/>
-      <c r="G11" s="50"/>
-      <c r="H11" s="53"/>
+      <c r="F11" s="48"/>
+      <c r="G11" s="48"/>
+      <c r="H11" s="51"/>
       <c r="I11" s="11"/>
       <c r="J11" s="6"/>
       <c r="K11" s="12"/>
@@ -1538,9 +1534,9 @@
       <c r="C12" s="6"/>
       <c r="D12" s="12"/>
       <c r="E12" s="11"/>
-      <c r="F12" s="50"/>
-      <c r="G12" s="50"/>
-      <c r="H12" s="53"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="48"/>
+      <c r="H12" s="51"/>
       <c r="I12" s="9" t="s">
         <v>58</v>
       </c>
@@ -1561,9 +1557,9 @@
       <c r="C13" s="6"/>
       <c r="D13" s="12"/>
       <c r="E13" s="11"/>
-      <c r="F13" s="50"/>
-      <c r="G13" s="50"/>
-      <c r="H13" s="53"/>
+      <c r="F13" s="48"/>
+      <c r="G13" s="48"/>
+      <c r="H13" s="51"/>
       <c r="I13" s="11"/>
       <c r="J13" s="5"/>
       <c r="K13" s="12"/>
@@ -1582,9 +1578,9 @@
       <c r="C14" s="6"/>
       <c r="D14" s="12"/>
       <c r="E14" s="11"/>
-      <c r="F14" s="50"/>
-      <c r="G14" s="50"/>
-      <c r="H14" s="53"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="48"/>
+      <c r="H14" s="51"/>
       <c r="I14" s="11" t="s">
         <v>58</v>
       </c>
@@ -1605,9 +1601,9 @@
       <c r="C15" s="6"/>
       <c r="D15" s="12"/>
       <c r="E15" s="11"/>
-      <c r="F15" s="50"/>
-      <c r="G15" s="50"/>
-      <c r="H15" s="53"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="48"/>
+      <c r="H15" s="51"/>
       <c r="I15" s="11"/>
       <c r="J15" s="6"/>
       <c r="K15" s="12"/>
@@ -1626,9 +1622,9 @@
       <c r="C16" s="6"/>
       <c r="D16" s="12"/>
       <c r="E16" s="11"/>
-      <c r="F16" s="50"/>
-      <c r="G16" s="50"/>
-      <c r="H16" s="53"/>
+      <c r="F16" s="48"/>
+      <c r="G16" s="48"/>
+      <c r="H16" s="51"/>
       <c r="I16" s="11"/>
       <c r="J16" s="6" t="s">
         <v>58</v>
@@ -1651,9 +1647,9 @@
       <c r="C17" s="6"/>
       <c r="D17" s="12"/>
       <c r="E17" s="11"/>
-      <c r="F17" s="50"/>
-      <c r="G17" s="50"/>
-      <c r="H17" s="53"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="51"/>
       <c r="I17" s="11"/>
       <c r="J17" s="6" t="s">
         <v>58</v>
@@ -1671,9 +1667,9 @@
       <c r="C18" s="6"/>
       <c r="D18" s="12"/>
       <c r="E18" s="11"/>
-      <c r="F18" s="50"/>
-      <c r="G18" s="50"/>
-      <c r="H18" s="53"/>
+      <c r="F18" s="48"/>
+      <c r="G18" s="48"/>
+      <c r="H18" s="51"/>
       <c r="I18" s="11"/>
       <c r="J18" s="6"/>
       <c r="K18" s="10"/>
@@ -1692,9 +1688,9 @@
       <c r="C19" s="6"/>
       <c r="D19" s="12"/>
       <c r="E19" s="11"/>
-      <c r="F19" s="50"/>
-      <c r="G19" s="50"/>
-      <c r="H19" s="53"/>
+      <c r="F19" s="48"/>
+      <c r="G19" s="48"/>
+      <c r="H19" s="51"/>
       <c r="I19" s="11"/>
       <c r="J19" s="6"/>
       <c r="K19" s="12" t="s">
@@ -1725,9 +1721,9 @@
       <c r="C20" s="6"/>
       <c r="D20" s="12"/>
       <c r="E20" s="11"/>
-      <c r="F20" s="50"/>
-      <c r="G20" s="50"/>
-      <c r="H20" s="53"/>
+      <c r="F20" s="48"/>
+      <c r="G20" s="48"/>
+      <c r="H20" s="51"/>
       <c r="I20" s="11"/>
       <c r="J20" s="6"/>
       <c r="K20" s="12"/>
@@ -1744,9 +1740,9 @@
       <c r="C21" s="6"/>
       <c r="D21" s="12"/>
       <c r="E21" s="11"/>
-      <c r="F21" s="50"/>
-      <c r="G21" s="50"/>
-      <c r="H21" s="53"/>
+      <c r="F21" s="48"/>
+      <c r="G21" s="48"/>
+      <c r="H21" s="51"/>
       <c r="I21" s="11"/>
       <c r="J21" s="6"/>
       <c r="K21" s="12"/>
@@ -1765,9 +1761,9 @@
       <c r="C22" s="6"/>
       <c r="D22" s="12"/>
       <c r="E22" s="11"/>
-      <c r="F22" s="50"/>
-      <c r="G22" s="50"/>
-      <c r="H22" s="53"/>
+      <c r="F22" s="48"/>
+      <c r="G22" s="48"/>
+      <c r="H22" s="51"/>
       <c r="I22" s="11"/>
       <c r="J22" s="6"/>
       <c r="K22" s="12"/>
@@ -1788,9 +1784,9 @@
       <c r="C23" s="6"/>
       <c r="D23" s="12"/>
       <c r="E23" s="11"/>
-      <c r="F23" s="50"/>
-      <c r="G23" s="50"/>
-      <c r="H23" s="53"/>
+      <c r="F23" s="48"/>
+      <c r="G23" s="48"/>
+      <c r="H23" s="51"/>
       <c r="I23" s="11"/>
       <c r="J23" s="6"/>
       <c r="K23" s="12"/>
@@ -1807,9 +1803,9 @@
       <c r="C24" s="30"/>
       <c r="D24" s="31"/>
       <c r="E24" s="29"/>
-      <c r="F24" s="50"/>
-      <c r="G24" s="50"/>
-      <c r="H24" s="53"/>
+      <c r="F24" s="48"/>
+      <c r="G24" s="48"/>
+      <c r="H24" s="51"/>
       <c r="I24" s="29"/>
       <c r="J24" s="30"/>
       <c r="K24" s="31"/>
@@ -1828,9 +1824,9 @@
       <c r="C25" s="30"/>
       <c r="D25" s="31"/>
       <c r="E25" s="29"/>
-      <c r="F25" s="50"/>
-      <c r="G25" s="50"/>
-      <c r="H25" s="53"/>
+      <c r="F25" s="48"/>
+      <c r="G25" s="48"/>
+      <c r="H25" s="51"/>
       <c r="I25" s="29"/>
       <c r="J25" s="30"/>
       <c r="K25" s="31"/>
@@ -1847,9 +1843,9 @@
       <c r="C26" s="30"/>
       <c r="D26" s="31"/>
       <c r="E26" s="29"/>
-      <c r="F26" s="50"/>
-      <c r="G26" s="50"/>
-      <c r="H26" s="53"/>
+      <c r="F26" s="48"/>
+      <c r="G26" s="48"/>
+      <c r="H26" s="51"/>
       <c r="I26" s="29"/>
       <c r="J26" s="30"/>
       <c r="K26" s="31"/>
@@ -1868,9 +1864,9 @@
       <c r="C27" s="14"/>
       <c r="D27" s="15"/>
       <c r="E27" s="13"/>
-      <c r="F27" s="51"/>
-      <c r="G27" s="51"/>
-      <c r="H27" s="54"/>
+      <c r="F27" s="49"/>
+      <c r="G27" s="49"/>
+      <c r="H27" s="52"/>
       <c r="I27" s="13"/>
       <c r="J27" s="14"/>
       <c r="K27" s="15"/>
@@ -1883,11 +1879,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="O7:Q7"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="F9:F27"/>
-    <mergeCell ref="G9:G27"/>
-    <mergeCell ref="H9:H27"/>
     <mergeCell ref="A1:N1"/>
     <mergeCell ref="B3:K3"/>
     <mergeCell ref="B4:K4"/>
@@ -1895,6 +1886,11 @@
     <mergeCell ref="E7:G7"/>
     <mergeCell ref="I7:K7"/>
     <mergeCell ref="L7:N7"/>
+    <mergeCell ref="O7:Q7"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="F9:F27"/>
+    <mergeCell ref="G9:G27"/>
+    <mergeCell ref="H9:H27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="91" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -1924,11 +1920,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
@@ -2144,8 +2140,8 @@
   </sheetPr>
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2156,11 +2152,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
@@ -2370,6 +2366,71 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Self_Registration_Enabled xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Student_Groups xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Student_Groups>
+    <Distribution_Groups xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <AppVersion xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Invited_Teachers xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Templates xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Has_Teacher_Only_SectionGroup xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <CultureName xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <LMS_Mappings xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Invited_Students xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <FolderType xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Teachers xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Teachers>
+    <TeamsChannelId xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <IsNotebookLocked xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Is_Collaboration_Space_Locked xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Teams_Channel_Section_Location xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Math_Settings xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Owner xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Owner>
+    <Students xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Students>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="3fb344db-9a83-4925-8457-d4a81a8233b7" xsi:nil="true"/>
+    <NotebookType xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <DefaultSectionNames xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004EEFC8B7315DA4449F69FE97A704FE57" ma:contentTypeVersion="35" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="c91a1a7a62e987314df808fa39da4b34">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cc3645a1-58b5-4da5-acb4-f681c13b5e81" xmlns:ns3="3fb344db-9a83-4925-8457-d4a81a8233b7" xmlns:ns4="52c6fd7a-766c-4f84-9f35-2a37be325271" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5e3023738844047246cab05fc3830165" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="cc3645a1-58b5-4da5-acb4-f681c13b5e81"/>
@@ -2823,72 +2884,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Self_Registration_Enabled xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Student_Groups xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Student_Groups>
-    <Distribution_Groups xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <AppVersion xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Invited_Teachers xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Templates xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Has_Teacher_Only_SectionGroup xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <CultureName xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <LMS_Mappings xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Invited_Students xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <FolderType xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Teachers xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Teachers>
-    <TeamsChannelId xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <IsNotebookLocked xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Is_Collaboration_Space_Locked xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Teams_Channel_Section_Location xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Math_Settings xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Owner xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Owner>
-    <Students xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Students>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="3fb344db-9a83-4925-8457-d4a81a8233b7" xsi:nil="true"/>
-    <NotebookType xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <DefaultSectionNames xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE473839-D414-4B78-82BC-08E64CD93726}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE303A41-7D70-49B7-87A8-C6207A042BC3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="52c6fd7a-766c-4f84-9f35-2a37be325271"/>
+    <ds:schemaRef ds:uri="3fb344db-9a83-4925-8457-d4a81a8233b7"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{05539879-8A52-4B74-9FF2-F471F780BCE4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2906,23 +2921,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE303A41-7D70-49B7-87A8-C6207A042BC3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="52c6fd7a-766c-4f84-9f35-2a37be325271"/>
-    <ds:schemaRef ds:uri="3fb344db-9a83-4925-8457-d4a81a8233b7"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE473839-D414-4B78-82BC-08E64CD93726}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>